<commit_message>
update products and translations
</commit_message>
<xml_diff>
--- a/public/uploads/sheetExcel/newProducts.xlsx
+++ b/public/uploads/sheetExcel/newProducts.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8640"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>amount</t>
   </si>
@@ -40,9 +40,6 @@
     <t>desc_en</t>
   </si>
   <si>
-    <t>kilo</t>
-  </si>
-  <si>
     <t xml:space="preserve">حماده </t>
   </si>
   <si>
@@ -55,12 +52,6 @@
     <t>description</t>
   </si>
   <si>
-    <t>unit_ar</t>
-  </si>
-  <si>
-    <t>unit_en</t>
-  </si>
-  <si>
     <t>type_ar</t>
   </si>
   <si>
@@ -73,9 +64,6 @@
     <t>kars</t>
   </si>
   <si>
-    <t>كيلو</t>
-  </si>
-  <si>
     <t>brand</t>
   </si>
   <si>
@@ -97,16 +85,13 @@
     <t>desc test</t>
   </si>
   <si>
-    <t>lite</t>
-  </si>
-  <si>
-    <t>لت</t>
-  </si>
-  <si>
     <t>حقن</t>
   </si>
   <si>
     <t>ghj</t>
+  </si>
+  <si>
+    <t>discount</t>
   </si>
 </sst>
 </file>
@@ -221,7 +206,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -256,7 +241,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -465,10 +450,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M3"/>
+  <dimension ref="A1:L3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -477,11 +462,12 @@
     <col min="2" max="3" width="9.140625" style="4"/>
     <col min="4" max="4" width="20.7109375" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.140625" style="4"/>
+    <col min="9" max="9" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>0</v>
@@ -508,21 +494,18 @@
         <v>7</v>
       </c>
       <c r="J1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>16</v>
-      </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B2" s="4">
         <v>77</v>
@@ -537,33 +520,30 @@
         <v>1</v>
       </c>
       <c r="F2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" t="s">
         <v>9</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>10</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>11</v>
       </c>
-      <c r="I2" t="s">
-        <v>12</v>
-      </c>
-      <c r="J2" t="s">
-        <v>19</v>
+      <c r="J2">
+        <v>1</v>
       </c>
       <c r="K2" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="L2" t="s">
-        <v>17</v>
-      </c>
-      <c r="M2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
         <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
-        <v>22</v>
       </c>
       <c r="B3" s="4">
         <v>14</v>
@@ -578,28 +558,25 @@
         <v>1</v>
       </c>
       <c r="F3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H3" t="s">
+        <v>21</v>
+      </c>
+      <c r="I3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J3">
+        <v>2</v>
+      </c>
+      <c r="K3" t="s">
         <v>23</v>
       </c>
-      <c r="G3" t="s">
+      <c r="L3" t="s">
         <v>24</v>
-      </c>
-      <c r="H3" t="s">
-        <v>25</v>
-      </c>
-      <c r="I3" t="s">
-        <v>26</v>
-      </c>
-      <c r="J3" t="s">
-        <v>28</v>
-      </c>
-      <c r="K3" t="s">
-        <v>27</v>
-      </c>
-      <c r="L3" t="s">
-        <v>29</v>
-      </c>
-      <c r="M3" t="s">
-        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>